<commit_message>
Update item code test
</commit_message>
<xml_diff>
--- a/municipal_finance/fixtures/tests/update/item_schema.xlsx
+++ b/municipal_finance/fixtures/tests/update/item_schema.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="A7" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t xml:space="preserve">MSCOA Account (version 6.8) linking to A1 schedule sheets</t>
   </si>
@@ -37,13 +37,19 @@
 A1 schedule Code description</t>
   </si>
   <si>
-    <t xml:space="preserve">A4</t>
+    <t xml:space="preserve">A7</t>
   </si>
   <si>
     <t xml:space="preserve">0300</t>
   </si>
   <si>
     <t xml:space="preserve">Exchange Revenue / Service charges - Electricity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exchange Revenue / New Item Code</t>
   </si>
 </sst>
 </file>
@@ -58,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -255,13 +262,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -363,6 +370,17 @@
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>